<commit_message>
new results for serum generated
</commit_message>
<xml_diff>
--- a/EVGLMresults.xlsx
+++ b/EVGLMresults.xlsx
@@ -15,9 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">microRNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coefficient.estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard.deviation</t>
   </si>
   <si>
     <t xml:space="preserve">p.value</t>
@@ -542,492 +548,864 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
+        <v>-0.0763052271519631</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.0469123999986337</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
+        <v>0.10033794990673</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.0510108623320968</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
+        <v>-0.0670021225634853</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.0783689322723704</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
+        <v>-0.0705368429346508</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.104322045729845</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
+        <v>-0.0604666234345592</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.120907999878529</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
+        <v>-0.0561617628829433</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.121501405680239</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
+        <v>-0.0554653492159775</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.128261400406771</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
+        <v>-0.148935707213245</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.141254446544038</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
+        <v>-0.084668096032864</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.144394706300263</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
+        <v>-0.0779037691436003</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.15519509437638</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
+        <v>-0.0584013075596875</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.155706891450863</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
+        <v>-0.0420657040715558</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.156853858751976</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
+        <v>-0.0494180754129195</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.179824627724122</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15" t="n">
+        <v>-0.0486824963578774</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.188681686004119</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" t="n">
+        <v>-0.065561781402192</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.199918638880457</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17" t="n">
+        <v>-0.0395532755819045</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.200462492438037</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B18" t="n">
+        <v>-0.0721404039918988</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.213645310126956</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19" t="n">
+        <v>-0.0509741272935522</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.216288815097393</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B20" t="n">
+        <v>-0.049483371211158</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.232908563470193</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B21" t="n">
+        <v>-0.0444286046878637</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.238292358011728</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B22" t="n">
+        <v>-0.048968729734294</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.241294292682971</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B23" t="n">
+        <v>-0.0543378566316912</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.285532128278508</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B24" t="n">
+        <v>-0.0432736133160775</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.288416975024557</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B25" t="n">
+        <v>-0.0364013002509875</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.292148064644972</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" t="n">
+        <v>-0.0349417210926487</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D26" t="n">
         <v>0.299676777693926</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" t="n">
+        <v>-0.0328797587547415</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.323416250784635</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" t="n">
+        <v>-0.0212038487805496</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.332737354261762</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B29" t="n">
+        <v>-0.041883650622317</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.332950630532802</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B30" t="n">
+        <v>-0.0500639422743185</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D30" t="n">
         <v>0.339671560736274</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B31" t="n">
+        <v>-0.0355943380605704</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.352675491257553</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B32" t="n">
+        <v>-0.0252079200497155</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.354622377346818</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B33" t="n">
+        <v>-0.0279185664179544</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.37650189050805</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" t="n">
+        <v>-0.0278728594887648</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.39221085575803</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B35" t="n">
+        <v>-0.0367090623983753</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.395462340292157</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B36" t="n">
+        <v>-0.0353908986131646</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D36" t="n">
         <v>0.404377310515613</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B37" t="n">
+        <v>-0.0339265137663662</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D37" t="n">
         <v>0.409151907775059</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B38" t="n">
+        <v>-0.0516418237771288</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D38" t="n">
         <v>0.411136221741852</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B39" t="n">
+        <v>-0.0461392575220597</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D39" t="n">
         <v>0.412775177630416</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B40" t="n">
+        <v>-0.0173510820931784</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.441867808472827</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B41" t="n">
+        <v>-0.0385285867550733</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.44598756010407</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B42" t="n">
+        <v>-0.0238794242618883</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.449436709404728</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B43" t="n">
+        <v>-0.0258276465498037</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.477610205824617</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B44" t="n">
+        <v>-0.0274843857977052</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D44" t="n">
         <v>0.492649308630602</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B45" t="n">
+        <v>-0.0337216484307791</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.493846525208562</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B46" t="n">
+        <v>-0.031618543711765</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D46" t="n">
         <v>0.497805736417223</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B47" t="n">
+        <v>-0.0194091004097648</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D47" t="n">
         <v>0.499465683635988</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B48" t="n">
+        <v>-0.0428132488903195</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D48" t="n">
         <v>0.52850230586972</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B49" t="n">
+        <v>-0.0364650457578673</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D49" t="n">
         <v>0.547717374272948</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B50" t="n">
+        <v>0.0156003580378038</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D50" t="n">
         <v>0.564710340615262</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B51" t="n">
+        <v>-0.0284209650370402</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D51" t="n">
         <v>0.566866712575584</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B52" t="n">
+        <v>-0.0222945556673554</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D52" t="n">
         <v>0.585601264778982</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B53" t="n">
+        <v>0.0146636746639555</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D53" t="n">
         <v>0.594346840731841</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B54" t="n">
+        <v>-0.0400598306576633</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.598134258139485</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B55" t="n">
+        <v>-0.0323433640209836</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.630230753700555</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B56" t="n">
+        <v>-0.0190941353475554</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.693752737715738</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B57" t="n">
+        <v>-0.0117897634023689</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.766627159196817</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B58" t="n">
+        <v>-0.0237894073887506</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D58" t="n">
         <v>0.772286988709727</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B59" t="n">
+        <v>0.00676424536639544</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D59" t="n">
         <v>0.849766115822535</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B60" t="n">
+        <v>-0.0040742252784196</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D60" t="n">
         <v>0.883276262106089</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B61" t="n">
+        <v>0.00372214670965654</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.883583541473916</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B62" t="n">
+        <v>-0.00565383103112839</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.0374806734950515</v>
+      </c>
+      <c r="D62" t="n">
         <v>0.976872451359486</v>
       </c>
     </row>
@@ -1052,492 +1430,864 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="n">
+        <v>-0.258951327648078</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.100955679803525</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.0115933715523465</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="n">
+        <v>-0.394398268721543</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.171708786931031</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.0234184345562587</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
+        <v>-0.353762341210877</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.156304104574164</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.0254773684464722</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="n">
+        <v>-0.407976937534661</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.182350931194948</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.0271759695197116</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="n">
+        <v>-0.299476972190242</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.134787617936956</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.0282341517472581</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B7" t="n">
+        <v>0.166370887077954</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0750541478737976</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.0285952884274468</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
+        <v>-0.323522320641329</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.149604850127314</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.0326316593479957</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
+        <v>-0.252068676596143</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.118505654474348</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.0355335026330893</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10" t="n">
+        <v>0.40512488191822</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.197963131939006</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.0429707653763255</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="n">
+        <v>-0.266773763805851</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1322255102074</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.0459446047648329</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" t="n">
+        <v>-0.322439953646661</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.163194508685278</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.0505514478120755</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" t="n">
+        <v>0.227915225389179</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.122076556557597</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.0644282163969725</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" t="n">
+        <v>-0.0891331238469593</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0479278109921588</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.0654561958831707</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
+        <v>-0.348857674419955</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.188339920615496</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.0665283845942896</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" t="n">
+        <v>0.332476097811617</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.203630010100573</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.105234022097655</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B17" t="n">
+        <v>0.23250983397156</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.156927743026904</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.141148488261695</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" t="n">
+        <v>-0.219793615792888</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.152204134938873</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.151414441023447</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
+        <v>-0.145380446791152</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.100919070477466</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.152401413329872</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" t="n">
+        <v>-0.176461165068819</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.147198883847461</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.233051237457461</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="n">
+        <v>-0.205650339394867</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.187235183205428</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.274324885000376</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B22" t="n">
+        <v>-0.0716287252628522</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0660202589945298</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.280193188978099</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B23" t="n">
+        <v>-0.104730299462865</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0965601382117368</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.280342527312192</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
+        <v>-0.158873646200483</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.152317720493298</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.299098126050568</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" t="n">
+        <v>-0.191414757904197</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.183682665284889</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.299534712693653</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B26" t="n">
+        <v>0.0882901234465362</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0868149389200065</v>
+      </c>
+      <c r="D26" t="n">
         <v>0.311273561544261</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" t="n">
+        <v>0.110905842805974</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.111435941019205</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.321689623549303</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B28" t="n">
+        <v>0.178113542974048</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.183192650939163</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.332937062629686</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B29" t="n">
+        <v>-0.190780357189742</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.196931197164489</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.33467724031008</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" t="n">
+        <v>-0.0922909338704116</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0960964304780509</v>
+      </c>
+      <c r="D30" t="n">
         <v>0.338851945101033</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
+        <v>0.147429657314894</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.155556623413392</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.345224124293282</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B32" t="n">
+        <v>-0.173667074513425</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.189030827437811</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.360146582947162</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B33" t="n">
+        <v>-0.205750321315987</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.236026302146126</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.385158405950049</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" t="n">
+        <v>0.091591350521328</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.105498840882915</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.387091658070651</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" t="n">
+        <v>-0.0950040387726264</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.111318114409138</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.395170714766239</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B36" t="n">
+        <v>-0.216481745328884</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.257608852588407</v>
+      </c>
+      <c r="D36" t="n">
         <v>0.402440637736626</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B37" t="n">
+        <v>-0.115402564186821</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.14446456067878</v>
+      </c>
+      <c r="D37" t="n">
         <v>0.426021786136279</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B38" t="n">
+        <v>0.103448677494892</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.134041775603845</v>
+      </c>
+      <c r="D38" t="n">
         <v>0.441823337857637</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B39" t="n">
+        <v>-0.133017398665326</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.17337487284305</v>
+      </c>
+      <c r="D39" t="n">
         <v>0.444506997833536</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B40" t="n">
+        <v>0.0193916498001613</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0263321423814016</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.462958743805033</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B41" t="n">
+        <v>-0.0354198793170126</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.051483885055862</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.492838865516242</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B42" t="n">
+        <v>-0.131675055306126</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.195368488894445</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.501662913492545</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B43" t="n">
+        <v>0.126612137391757</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.190838926652202</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.508358582700698</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B44" t="n">
+        <v>0.0161208588778511</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0250311902733534</v>
+      </c>
+      <c r="D44" t="n">
         <v>0.520826808786506</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B45" t="n">
+        <v>-0.092252104403152</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.145499852133536</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.527305824662236</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B46" t="n">
+        <v>0.0536124888081878</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.0963632987130167</v>
+      </c>
+      <c r="D46" t="n">
         <v>0.579037844173671</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B47" t="n">
+        <v>0.0529423486123759</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0964705426751755</v>
+      </c>
+      <c r="D47" t="n">
         <v>0.584202350886741</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B48" t="n">
+        <v>0.0788369889026203</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.150352242104167</v>
+      </c>
+      <c r="D48" t="n">
         <v>0.60103663043493</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B49" t="n">
+        <v>0.0543680766162146</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.106941895911069</v>
+      </c>
+      <c r="D49" t="n">
         <v>0.612146095873462</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B50" t="n">
+        <v>0.0642888221274042</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.135300146401151</v>
+      </c>
+      <c r="D50" t="n">
         <v>0.635568472905244</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B51" t="n">
+        <v>-0.0862360054173692</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.181641552886474</v>
+      </c>
+      <c r="D51" t="n">
         <v>0.635851189441975</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B52" t="n">
+        <v>-0.13152900527624</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.292789237302091</v>
+      </c>
+      <c r="D52" t="n">
         <v>0.654105671903513</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B53" t="n">
+        <v>-0.0871025162964395</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.196005949994992</v>
+      </c>
+      <c r="D53" t="n">
         <v>0.657590702985755</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B54" t="n">
+        <v>-0.0444307347738558</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.141087036842489</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.753390289603566</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B55" t="n">
+        <v>-0.0234878068779793</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0754250255723894</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.756050936208635</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B56" t="n">
+        <v>-0.0136012128146742</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0446534036570745</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.761220256177671</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B57" t="n">
+        <v>0.0323625090679225</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.114068422580879</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.777137330333315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B58" t="n">
+        <v>0.0358609800725144</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.141425798016166</v>
+      </c>
+      <c r="D58" t="n">
         <v>0.800278609787603</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B59" t="n">
+        <v>0.00991973204926727</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0434644490094733</v>
+      </c>
+      <c r="D59" t="n">
         <v>0.819872112292151</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B60" t="n">
+        <v>-0.0300921661170291</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.163240953876681</v>
+      </c>
+      <c r="D60" t="n">
         <v>0.854067037910173</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B61" t="n">
+        <v>0.000105190053618457</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.193020156850397</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.999566113553403</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B62" t="n">
+        <v>0.0000723447881021558</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.140024572618724</v>
+      </c>
+      <c r="D62" t="n">
         <v>0.999588654200105</v>
       </c>
     </row>
@@ -1562,492 +2312,864 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="n">
+        <v>-0.246017579632504</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0983720523565027</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.0137841984984543</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
+        <v>-0.564231201667572</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.227809333500032</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.014699872628028</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" t="n">
+        <v>-0.405661799476967</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.171349505317142</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.0195662520862052</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" t="n">
+        <v>-0.33299494489613</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.142543121566335</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.0212030105081464</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B6" t="n">
+        <v>0.177533173480202</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0779409922663357</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.0245706724133968</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
+        <v>-0.334264837877482</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.155728482620262</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.0339191552565176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
+        <v>-0.22821567867805</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.111144183710231</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.0422892116424133</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
+        <v>-0.294522505565298</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.146519711969838</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.0467385086878411</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10" t="n">
+        <v>0.383792434194368</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.194327825650077</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.0506465294844244</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" t="n">
+        <v>0.287126544916958</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.147680278420714</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.0542872189237856</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="n">
+        <v>-0.0949043390664925</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0508698758903222</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.0646195573556745</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B13" t="n">
+        <v>-0.281895140376555</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.151179945820018</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.0647603853318421</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" t="n">
+        <v>-0.218913246130673</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.119552625054419</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.0696515073390415</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" t="n">
+        <v>0.460613497157691</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.2515735659266</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.0696776694541448</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" t="n">
+        <v>0.367983926218481</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.206302119772561</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.0770850063312525</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n">
+        <v>-0.312158168785352</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.178740773685463</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.0833834587416726</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" t="n">
+        <v>-0.171721043969404</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0992654115350651</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.0863046162796253</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
+        <v>0.242102937248176</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.141530366958767</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.0898266682045913</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" t="n">
+        <v>0.231441135118057</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.13713700845308</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.0941628948528165</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" t="n">
+        <v>0.249797351429648</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.167426944105893</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.138419502096863</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" t="n">
+        <v>-0.227180715764979</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.154342533070782</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.143748870938588</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" t="n">
+        <v>-0.192401791975094</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.132568037897244</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.149383240570644</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" t="n">
+        <v>0.243454142454398</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.194137457740883</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.212352439227927</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" t="n">
+        <v>0.190801639780719</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.156640348969051</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.225662520015024</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" t="n">
+        <v>-0.266049508667092</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.218997185661163</v>
+      </c>
+      <c r="D26" t="n">
         <v>0.226889034909796</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B27" t="n">
+        <v>-0.250209035684544</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.207583521719713</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.230524569508218</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="n">
+        <v>-0.23201846844974</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.199755672250185</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.247818480146041</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29" t="n">
+        <v>-0.232069976930907</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.205077950625962</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.260128875620986</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" t="n">
+        <v>0.226542202962918</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.207537448470885</v>
+      </c>
+      <c r="D30" t="n">
         <v>0.277283014706285</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B31" t="n">
+        <v>-0.0731552492123801</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0674331114430182</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.280234732411266</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
+        <v>-0.116412720276773</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.109833447859149</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.291391001501624</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B33" t="n">
+        <v>-0.0867477118019402</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0858453231994032</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.314353335027599</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B34" t="n">
+        <v>0.0738329507461105</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0816161407774001</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.367532913418584</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" t="n">
+        <v>-0.113011988700372</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.125303702348484</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.368976404624627</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B36" t="n">
+        <v>-0.172357781441202</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.191605218112843</v>
+      </c>
+      <c r="D36" t="n">
         <v>0.370225279120383</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B37" t="n">
+        <v>0.165192512826169</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.195975245998127</v>
+      </c>
+      <c r="D37" t="n">
         <v>0.401004877757143</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="n">
+        <v>-0.182967120835435</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.217430918729944</v>
+      </c>
+      <c r="D38" t="n">
         <v>0.40180187182334</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B39" t="n">
+        <v>-0.0446291211149562</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.0571295081767383</v>
+      </c>
+      <c r="D39" t="n">
         <v>0.436280928353576</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B40" t="n">
+        <v>-0.126981379063558</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.167667708953629</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.450382139807939</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="n">
+        <v>0.113253202488209</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.151518775342546</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.456302515854847</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B42" t="n">
+        <v>-0.189897007350177</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.256081226711238</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.459858778539291</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B43" t="n">
+        <v>0.0607107396470452</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0857246028882516</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.480237563313218</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B44" t="n">
+        <v>0.0177223896354788</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0271171427418133</v>
+      </c>
+      <c r="D44" t="n">
         <v>0.514695622074003</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" t="n">
+        <v>0.0168932100622719</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.0259333269676264</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.516070765044869</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B46" t="n">
+        <v>0.127373885631913</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.205867034250684</v>
+      </c>
+      <c r="D46" t="n">
         <v>0.537314464503001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B47" t="n">
+        <v>-0.132833449775561</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.215417476144703</v>
+      </c>
+      <c r="D47" t="n">
         <v>0.538685369226523</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B48" t="n">
+        <v>-0.0849811266740541</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.147426649949108</v>
+      </c>
+      <c r="D48" t="n">
         <v>0.565441466816507</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B49" t="n">
+        <v>-0.105204489166354</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.224688836913596</v>
+      </c>
+      <c r="D49" t="n">
         <v>0.640503694557011</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B50" t="n">
+        <v>-0.147311074139622</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.35827249868693</v>
+      </c>
+      <c r="D50" t="n">
         <v>0.681706160394105</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B51" t="n">
+        <v>-0.0238979035541535</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.0597178726313914</v>
+      </c>
+      <c r="D51" t="n">
         <v>0.68975987665757</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B52" t="n">
+        <v>-0.0421875922536895</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.136963902084974</v>
+      </c>
+      <c r="D52" t="n">
         <v>0.758619676006941</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" t="n">
+        <v>0.0316541562231578</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.104632378547285</v>
+      </c>
+      <c r="D53" t="n">
         <v>0.762791886508996</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B54" t="n">
+        <v>-0.0507297473477109</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.19479807469331</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.794999818667379</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B55" t="n">
+        <v>0.0237069516679031</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.10192556922259</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.816489036577625</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B56" t="n">
+        <v>-0.0519430499631489</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.258250441193387</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.840945734343356</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B57" t="n">
+        <v>-0.00637492085386211</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.035526871043902</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.857905747014055</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B58" t="n">
+        <v>-0.0329602821395344</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.199966766570015</v>
+      </c>
+      <c r="D58" t="n">
         <v>0.869365624887629</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B59" t="n">
+        <v>-0.0307801763809465</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.201078990081861</v>
+      </c>
+      <c r="D59" t="n">
         <v>0.87860505152592</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B60" t="n">
+        <v>0.0107605859463177</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.102797455509316</v>
+      </c>
+      <c r="D60" t="n">
         <v>0.916812456195258</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61" t="n">
+        <v>0.00415355524487923</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.040883999452975</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.919254610294087</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B62" t="n">
+        <v>0.00915363957186925</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.151453746655061</v>
+      </c>
+      <c r="D62" t="n">
         <v>0.951910388413356</v>
       </c>
     </row>
@@ -2072,484 +3194,850 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="n">
+        <v>0.515028408149602</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.157305365749482</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.00139757141995545</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" t="n">
+        <v>0.44659940987466</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.138159070737969</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.00159786248074706</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" t="n">
+        <v>0.19045377129479</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0589351961955329</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.00160259495993448</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5" t="n">
+        <v>0.392582550531874</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.123407746501872</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.00188205679481958</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" t="n">
+        <v>0.366932300247328</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.116149200281331</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.00201796888742051</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="n">
+        <v>0.30183384056</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.104752773523864</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.00471801473549441</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" t="n">
+        <v>0.258714704159846</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0936690095821512</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.00668124839857033</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" t="n">
+        <v>0.364869356523869</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.134738035845257</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.00779350109882506</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" t="n">
+        <v>0.370579579047325</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.14014689997368</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.00932113647716857</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" t="n">
+        <v>0.322594513910633</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.128670571119148</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.0135555408933702</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" t="n">
+        <v>0.635776667747003</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.253874803288348</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.0136591935272184</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" t="n">
+        <v>0.334681691582255</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.139291605589631</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.0178586128073038</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="n">
+        <v>0.344503902104763</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.163565448923016</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.0373418698452233</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" t="n">
+        <v>0.342413482293668</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.181659910760811</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.0619435794568878</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B16" t="n">
+        <v>0.156082724635449</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0889420303703149</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.0819198344956856</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" t="n">
+        <v>0.162884812503849</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0945388643773125</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.0875640710775877</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n">
+        <v>0.256880537407976</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.156396227241</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.103194958269207</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="n">
+        <v>0.357360676582343</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.218655991916893</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.104896205983887</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
+        <v>-0.149917603745626</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0937097177518782</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.11236122287933</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B21" t="n">
+        <v>0.0865130919710721</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0564928389275608</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.128393417107548</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="n">
+        <v>0.128870791246848</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0936718561566443</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.171543900490626</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B23" t="n">
+        <v>-0.23049188841008</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.174660450055332</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.189548127758647</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" t="n">
+        <v>0.21277651967362</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.162556783429128</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.193142962412659</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B25" t="n">
+        <v>-0.056215191210046</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0434376454945668</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.198181313191974</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" t="n">
+        <v>0.105877890605968</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0822662429779459</v>
+      </c>
+      <c r="D26" t="n">
         <v>0.200651316137903</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B27" t="n">
+        <v>0.163800662871134</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.12732259807492</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.200829892152374</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" t="n">
+        <v>0.203550186945292</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.161415170342574</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.209826527414719</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B29" t="n">
+        <v>0.248792266526209</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.202080955672493</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.220756526112525</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" t="n">
+        <v>0.123299825175395</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.111459478121117</v>
+      </c>
+      <c r="D30" t="n">
         <v>0.270915862657672</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B31" t="n">
+        <v>0.204741836140257</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.186926571503232</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.275651440437258</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B32" t="n">
+        <v>0.252019310550381</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.238788015234305</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.293430952241878</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B33" t="n">
+        <v>0.101804247212524</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0989842331602398</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.305859406758408</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="n">
+        <v>0.223270125919901</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.220347471798054</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.313042988437528</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B35" t="n">
+        <v>0.149468285519394</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.147855379892862</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.314164144265529</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B36" t="n">
+        <v>-0.171699475055042</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.179012849810941</v>
+      </c>
+      <c r="D36" t="n">
         <v>0.339480051965394</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B37" t="n">
+        <v>0.21143440222555</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.221205766127167</v>
+      </c>
+      <c r="D37" t="n">
         <v>0.341147470403213</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B38" t="n">
+        <v>0.189563930943986</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.20217973905644</v>
+      </c>
+      <c r="D38" t="n">
         <v>0.350397530259494</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39" t="n">
+        <v>-0.0766639768694214</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.088780747142355</v>
+      </c>
+      <c r="D39" t="n">
         <v>0.389633416864539</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B40" t="n">
+        <v>-0.104981009798922</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.126078553826087</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.406745581854653</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" t="n">
+        <v>-0.0851499563702806</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.106812312946574</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.426968077288874</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B42" t="n">
+        <v>0.0128802079294336</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.0161903027998924</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.427918099428172</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B43" t="n">
+        <v>0.0124309642088046</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.015644142756302</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.428464158434437</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B44" t="n">
+        <v>0.0992838384510815</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.126113986089579</v>
+      </c>
+      <c r="D44" t="n">
         <v>0.432738302238531</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B45" t="n">
+        <v>-0.11769330524445</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.149560476835847</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.432928904809795</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" t="n">
+        <v>-0.0778000840590078</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.102862258913295</v>
+      </c>
+      <c r="D46" t="n">
         <v>0.450971465262665</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B47" t="n">
+        <v>-0.101754953534454</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.137912510108687</v>
+      </c>
+      <c r="D47" t="n">
         <v>0.462112279276798</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B48" t="n">
+        <v>-0.024458509649832</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0401949001773027</v>
+      </c>
+      <c r="D48" t="n">
         <v>0.544047038323306</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B49" t="n">
+        <v>0.123806872442572</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.216015782688411</v>
+      </c>
+      <c r="D49" t="n">
         <v>0.567660587831636</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B50" t="n">
+        <v>-0.0505041396806549</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.112715798909774</v>
+      </c>
+      <c r="D50" t="n">
         <v>0.654941155019984</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B51" t="n">
+        <v>-0.0559562264610314</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.126422657661321</v>
+      </c>
+      <c r="D51" t="n">
         <v>0.658870394267987</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B52" t="n">
+        <v>0.037521606794193</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.101651678015525</v>
+      </c>
+      <c r="D52" t="n">
         <v>0.712711624623493</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B53" t="n">
+        <v>-0.0361662735780244</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.11298171077179</v>
+      </c>
+      <c r="D53" t="n">
         <v>0.749462836396969</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B54" t="n">
+        <v>0.00850552877815013</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0275959380071587</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.758470232985477</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B55" t="n">
+        <v>0.0229231970001317</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.146120510774828</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.875613161917548</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B56" t="n">
+        <v>-0.0264931359947918</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.187782161089443</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.888047970969232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B57" t="n">
+        <v>-0.022483130941447</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.167025302120119</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.893154203267833</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B58" t="n">
+        <v>0.0145383841171041</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.120240503461609</v>
+      </c>
+      <c r="D58" t="n">
         <v>0.90397081942128</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B59" t="n">
+        <v>0.0053057231841713</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0522366281179571</v>
+      </c>
+      <c r="D59" t="n">
         <v>0.919272610935502</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B60" t="n">
+        <v>-0.00391512191909448</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0493211537681793</v>
+      </c>
+      <c r="D60" t="n">
         <v>0.936867014032249</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B61" t="n">
+        <v>-0.000159420773231722</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0398556312967697</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.996815376143195</v>
       </c>
     </row>

</xml_diff>